<commit_message>
Updated SC for testing
</commit_message>
<xml_diff>
--- a/SC 1.0.xlsx
+++ b/SC 1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephen.holwell\Desktop\Schedules\SC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randy.parsons\Desktop\Scheduling Stuff\SCH 1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14745" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="1178" sheetId="1" r:id="rId1"/>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,11 +1574,11 @@
       <c r="F20" s="7">
         <v>1039</v>
       </c>
-      <c r="G20" s="7">
-        <v>1</v>
-      </c>
-      <c r="H20" s="3">
+      <c r="G20" s="3">
         <v>2</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>27</v>
@@ -1617,10 +1617,10 @@
         <v>1039</v>
       </c>
       <c r="G21" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>27</v>
@@ -1659,10 +1659,10 @@
         <v>1039</v>
       </c>
       <c r="G22" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>27</v>
@@ -1701,10 +1701,10 @@
         <v>1039</v>
       </c>
       <c r="G23" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>27</v>
@@ -1743,10 +1743,10 @@
         <v>1039</v>
       </c>
       <c r="G24" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>27</v>
@@ -1785,10 +1785,10 @@
         <v>1038</v>
       </c>
       <c r="G25" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>17</v>
@@ -1829,10 +1829,10 @@
         <v>1038</v>
       </c>
       <c r="G26" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>17</v>
@@ -1873,10 +1873,10 @@
         <v>1038</v>
       </c>
       <c r="G27" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>17</v>
@@ -1917,10 +1917,10 @@
         <v>1038</v>
       </c>
       <c r="G28" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>17</v>
@@ -1961,10 +1961,10 @@
         <v>1038</v>
       </c>
       <c r="G29" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>17</v>
@@ -2005,10 +2005,10 @@
         <v>1038</v>
       </c>
       <c r="G30" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>17</v>
@@ -2049,10 +2049,10 @@
         <v>1038</v>
       </c>
       <c r="G31" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H31" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>17</v>
@@ -2093,10 +2093,10 @@
         <v>1038</v>
       </c>
       <c r="G32" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>17</v>
@@ -2137,10 +2137,10 @@
         <v>1101</v>
       </c>
       <c r="G33" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H33" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>17</v>
@@ -2181,10 +2181,10 @@
         <v>2160</v>
       </c>
       <c r="G34" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34" s="7" t="s">
         <v>17</v>
@@ -2225,10 +2225,10 @@
         <v>2160</v>
       </c>
       <c r="G35" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>17</v>
@@ -2269,10 +2269,10 @@
         <v>1060</v>
       </c>
       <c r="G36" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>17</v>
@@ -2313,10 +2313,10 @@
         <v>1038</v>
       </c>
       <c r="G37" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H37" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>17</v>
@@ -2355,10 +2355,10 @@
         <v>1038</v>
       </c>
       <c r="G38" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H38" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>17</v>
@@ -2397,10 +2397,10 @@
         <v>1038</v>
       </c>
       <c r="G39" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H39" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>17</v>
@@ -2439,10 +2439,10 @@
         <v>1038</v>
       </c>
       <c r="G40" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H40" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>17</v>
@@ -2481,10 +2481,10 @@
         <v>1038</v>
       </c>
       <c r="G41" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H41" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>17</v>
@@ -2523,10 +2523,10 @@
         <v>1038</v>
       </c>
       <c r="G42" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H42" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>17</v>
@@ -2565,10 +2565,10 @@
         <v>1038</v>
       </c>
       <c r="G43" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H43" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>17</v>
@@ -2607,10 +2607,10 @@
         <v>1038</v>
       </c>
       <c r="G44" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H44" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I44" s="7" t="s">
         <v>17</v>
@@ -2649,10 +2649,10 @@
         <v>1038</v>
       </c>
       <c r="G45" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H45" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>17</v>
@@ -2691,10 +2691,10 @@
         <v>1100</v>
       </c>
       <c r="G46" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H46" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>17</v>
@@ -2735,10 +2735,10 @@
         <v>1100</v>
       </c>
       <c r="G47" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H47" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>17</v>
@@ -2779,10 +2779,10 @@
         <v>2160</v>
       </c>
       <c r="G48" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H48" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>17</v>
@@ -2823,10 +2823,10 @@
         <v>2160</v>
       </c>
       <c r="G49" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H49" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>17</v>
@@ -2867,10 +2867,10 @@
         <v>2160</v>
       </c>
       <c r="G50" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H50" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I50" s="10" t="s">
         <v>17</v>
@@ -2911,10 +2911,10 @@
         <v>1039</v>
       </c>
       <c r="G51" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H51" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>27</v>
@@ -2955,10 +2955,10 @@
         <v>1039</v>
       </c>
       <c r="G52" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H52" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I52" s="7" t="s">
         <v>27</v>
@@ -2999,10 +2999,10 @@
         <v>1039</v>
       </c>
       <c r="G53" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H53" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I53" s="7" t="s">
         <v>27</v>
@@ -3043,10 +3043,10 @@
         <v>1039</v>
       </c>
       <c r="G54" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H54" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I54" s="7" t="s">
         <v>27</v>
@@ -3087,10 +3087,10 @@
         <v>1039</v>
       </c>
       <c r="G55" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H55" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>27</v>
@@ -3131,10 +3131,10 @@
         <v>1038</v>
       </c>
       <c r="G56" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H56" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I56" s="7" t="s">
         <v>17</v>
@@ -3175,10 +3175,10 @@
         <v>1038</v>
       </c>
       <c r="G57" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H57" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>17</v>
@@ -3219,10 +3219,10 @@
         <v>1038</v>
       </c>
       <c r="G58" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H58" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I58" s="7" t="s">
         <v>17</v>
@@ -3263,10 +3263,10 @@
         <v>1038</v>
       </c>
       <c r="G59" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H59" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>17</v>
@@ -3307,10 +3307,10 @@
         <v>1038</v>
       </c>
       <c r="G60" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H60" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>17</v>
@@ -3351,10 +3351,10 @@
         <v>1038</v>
       </c>
       <c r="G61" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H61" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>17</v>
@@ -3395,10 +3395,10 @@
         <v>1038</v>
       </c>
       <c r="G62" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H62" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I62" s="7" t="s">
         <v>17</v>
@@ -3439,10 +3439,10 @@
         <v>1038</v>
       </c>
       <c r="G63" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H63" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I63" s="7" t="s">
         <v>17</v>
@@ -3483,10 +3483,10 @@
         <v>1100</v>
       </c>
       <c r="G64" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H64" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>17</v>
@@ -3527,10 +3527,10 @@
         <v>1100</v>
       </c>
       <c r="G65" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H65" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>17</v>
@@ -3571,10 +3571,10 @@
         <v>2160</v>
       </c>
       <c r="G66" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H66" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>17</v>
@@ -3615,10 +3615,10 @@
         <v>2160</v>
       </c>
       <c r="G67" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H67" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I67" s="10" t="s">
         <v>17</v>
@@ -3659,10 +3659,10 @@
         <v>1038</v>
       </c>
       <c r="G68" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>17</v>
@@ -3701,10 +3701,10 @@
         <v>1038</v>
       </c>
       <c r="G69" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H69" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>17</v>
@@ -3743,10 +3743,10 @@
         <v>1038</v>
       </c>
       <c r="G70" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H70" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>17</v>
@@ -3785,10 +3785,10 @@
         <v>1038</v>
       </c>
       <c r="G71" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H71" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I71" s="7" t="s">
         <v>17</v>
@@ -3827,10 +3827,10 @@
         <v>1038</v>
       </c>
       <c r="G72" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H72" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>17</v>
@@ -3869,10 +3869,10 @@
         <v>1038</v>
       </c>
       <c r="G73" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H73" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>17</v>
@@ -3911,10 +3911,10 @@
         <v>1039</v>
       </c>
       <c r="G74" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H74" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I74" s="7" t="s">
         <v>27</v>
@@ -3953,10 +3953,10 @@
         <v>1039</v>
       </c>
       <c r="G75" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H75" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I75" s="7" t="s">
         <v>27</v>
@@ -3995,10 +3995,10 @@
         <v>1039</v>
       </c>
       <c r="G76" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H76" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I76" s="7" t="s">
         <v>27</v>
@@ -4037,10 +4037,10 @@
         <v>1039</v>
       </c>
       <c r="G77" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H77" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I77" s="7" t="s">
         <v>27</v>
@@ -4079,10 +4079,10 @@
         <v>1039</v>
       </c>
       <c r="G78" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H78" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I78" s="7" t="s">
         <v>27</v>
@@ -4121,10 +4121,10 @@
         <v>1100</v>
       </c>
       <c r="G79" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H79" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I79" s="7" t="s">
         <v>17</v>
@@ -4165,10 +4165,10 @@
         <v>1100</v>
       </c>
       <c r="G80" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H80" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I80" s="7" t="s">
         <v>17</v>
@@ -4209,10 +4209,10 @@
         <v>2160</v>
       </c>
       <c r="G81" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H81" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I81" s="7" t="s">
         <v>17</v>
@@ -4253,10 +4253,10 @@
         <v>2160</v>
       </c>
       <c r="G82" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H82" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>17</v>
@@ -7252,8 +7252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A158"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated again cuz we dumb
</commit_message>
<xml_diff>
--- a/SC 1.0.xlsx
+++ b/SC 1.0.xlsx
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I140" sqref="I140:I145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,8 +1404,8 @@
       <c r="H16" s="7">
         <v>1</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>27</v>
+      <c r="I16" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>28</v>
@@ -1448,8 +1448,8 @@
       <c r="H17" s="7">
         <v>1</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>27</v>
+      <c r="I17" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>28</v>
@@ -1492,8 +1492,8 @@
       <c r="H18" s="7">
         <v>1</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>27</v>
+      <c r="I18" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>28</v>
@@ -1536,8 +1536,8 @@
       <c r="H19" s="10">
         <v>1</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>27</v>
+      <c r="I19" s="27" t="s">
+        <v>17</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>28</v>
@@ -1580,8 +1580,8 @@
       <c r="H20" s="7">
         <v>1</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>27</v>
+      <c r="I20" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>28</v>
@@ -1622,8 +1622,8 @@
       <c r="H21" s="7">
         <v>1</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>27</v>
+      <c r="I21" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>28</v>
@@ -1664,8 +1664,8 @@
       <c r="H22" s="7">
         <v>1</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>27</v>
+      <c r="I22" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>28</v>
@@ -1706,8 +1706,8 @@
       <c r="H23" s="7">
         <v>1</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>27</v>
+      <c r="I23" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>28</v>
@@ -1748,8 +1748,8 @@
       <c r="H24" s="7">
         <v>1</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>27</v>
+      <c r="I24" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>28</v>
@@ -2916,8 +2916,8 @@
       <c r="H51" s="3">
         <v>1</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>27</v>
+      <c r="I51" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>28</v>
@@ -2960,8 +2960,8 @@
       <c r="H52" s="7">
         <v>1</v>
       </c>
-      <c r="I52" s="7" t="s">
-        <v>27</v>
+      <c r="I52" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J52" s="7" t="s">
         <v>28</v>
@@ -3004,8 +3004,8 @@
       <c r="H53" s="7">
         <v>1</v>
       </c>
-      <c r="I53" s="7" t="s">
-        <v>27</v>
+      <c r="I53" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J53" s="7" t="s">
         <v>28</v>
@@ -3048,8 +3048,8 @@
       <c r="H54" s="7">
         <v>1</v>
       </c>
-      <c r="I54" s="7" t="s">
-        <v>27</v>
+      <c r="I54" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J54" s="7" t="s">
         <v>28</v>
@@ -3092,8 +3092,8 @@
       <c r="H55" s="7">
         <v>1</v>
       </c>
-      <c r="I55" s="7" t="s">
-        <v>27</v>
+      <c r="I55" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J55" s="7" t="s">
         <v>28</v>
@@ -3916,8 +3916,8 @@
       <c r="H74" s="7">
         <v>1</v>
       </c>
-      <c r="I74" s="7" t="s">
-        <v>27</v>
+      <c r="I74" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J74" s="7" t="s">
         <v>28</v>
@@ -3958,8 +3958,8 @@
       <c r="H75" s="7">
         <v>1</v>
       </c>
-      <c r="I75" s="7" t="s">
-        <v>27</v>
+      <c r="I75" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J75" s="7" t="s">
         <v>28</v>
@@ -4000,8 +4000,8 @@
       <c r="H76" s="7">
         <v>1</v>
       </c>
-      <c r="I76" s="7" t="s">
-        <v>27</v>
+      <c r="I76" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J76" s="7" t="s">
         <v>28</v>
@@ -4042,8 +4042,8 @@
       <c r="H77" s="7">
         <v>1</v>
       </c>
-      <c r="I77" s="7" t="s">
-        <v>27</v>
+      <c r="I77" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J77" s="7" t="s">
         <v>28</v>
@@ -4084,8 +4084,8 @@
       <c r="H78" s="7">
         <v>1</v>
       </c>
-      <c r="I78" s="7" t="s">
-        <v>27</v>
+      <c r="I78" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J78" s="7" t="s">
         <v>28</v>
@@ -4742,8 +4742,8 @@
       <c r="H93" s="7">
         <v>1</v>
       </c>
-      <c r="I93" s="7" t="s">
-        <v>27</v>
+      <c r="I93" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>57</v>
@@ -4786,8 +4786,8 @@
       <c r="H94" s="7">
         <v>1</v>
       </c>
-      <c r="I94" s="7" t="s">
-        <v>27</v>
+      <c r="I94" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>57</v>
@@ -4830,8 +4830,8 @@
       <c r="H95" s="7">
         <v>1</v>
       </c>
-      <c r="I95" s="7" t="s">
-        <v>27</v>
+      <c r="I95" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J95" s="7" t="s">
         <v>57</v>
@@ -4874,8 +4874,8 @@
       <c r="H96" s="7">
         <v>1</v>
       </c>
-      <c r="I96" s="7" t="s">
-        <v>27</v>
+      <c r="I96" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J96" s="7" t="s">
         <v>57</v>
@@ -4918,8 +4918,8 @@
       <c r="H97" s="7">
         <v>1</v>
       </c>
-      <c r="I97" s="7" t="s">
-        <v>27</v>
+      <c r="I97" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J97" s="7" t="s">
         <v>57</v>
@@ -4962,8 +4962,8 @@
       <c r="H98" s="7">
         <v>1</v>
       </c>
-      <c r="I98" s="7" t="s">
-        <v>27</v>
+      <c r="I98" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J98" s="7" t="s">
         <v>57</v>
@@ -6398,8 +6398,8 @@
       <c r="H131" s="7">
         <v>1</v>
       </c>
-      <c r="I131" s="7" t="s">
-        <v>27</v>
+      <c r="I131" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J131" s="7" t="s">
         <v>28</v>
@@ -6442,8 +6442,8 @@
       <c r="H132" s="7">
         <v>1</v>
       </c>
-      <c r="I132" s="7" t="s">
-        <v>27</v>
+      <c r="I132" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J132" s="7" t="s">
         <v>28</v>
@@ -6486,8 +6486,8 @@
       <c r="H133" s="7">
         <v>1</v>
       </c>
-      <c r="I133" s="7" t="s">
-        <v>27</v>
+      <c r="I133" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J133" s="7" t="s">
         <v>28</v>
@@ -6530,8 +6530,8 @@
       <c r="H134" s="7">
         <v>1</v>
       </c>
-      <c r="I134" s="7" t="s">
-        <v>27</v>
+      <c r="I134" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J134" s="7" t="s">
         <v>28</v>
@@ -6574,8 +6574,8 @@
       <c r="H135" s="10">
         <v>1</v>
       </c>
-      <c r="I135" s="10" t="s">
-        <v>27</v>
+      <c r="I135" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J135" s="10" t="s">
         <v>28</v>
@@ -6828,8 +6828,8 @@
       <c r="H141" s="7">
         <v>1</v>
       </c>
-      <c r="I141" s="7" t="s">
-        <v>27</v>
+      <c r="I141" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J141" s="7" t="s">
         <v>28</v>
@@ -6872,8 +6872,8 @@
       <c r="H142" s="7">
         <v>1</v>
       </c>
-      <c r="I142" s="7" t="s">
-        <v>27</v>
+      <c r="I142" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J142" s="7" t="s">
         <v>28</v>
@@ -6916,8 +6916,8 @@
       <c r="H143" s="7">
         <v>1</v>
       </c>
-      <c r="I143" s="7" t="s">
-        <v>27</v>
+      <c r="I143" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J143" s="7" t="s">
         <v>28</v>
@@ -6960,8 +6960,8 @@
       <c r="H144" s="7">
         <v>1</v>
       </c>
-      <c r="I144" s="7" t="s">
-        <v>27</v>
+      <c r="I144" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J144" s="7" t="s">
         <v>28</v>
@@ -7004,8 +7004,8 @@
       <c r="H145" s="7">
         <v>1</v>
       </c>
-      <c r="I145" s="7" t="s">
-        <v>27</v>
+      <c r="I145" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="J145" s="7" t="s">
         <v>28</v>

</xml_diff>